<commit_message>
Salmonella and VTEC all instances
All currently in GenEpiO as instances.
</commit_message>
<xml_diff>
--- a/docs/campy.xlsx
+++ b/docs/campy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernanda.dorea\Documents\GitHub\HSO\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9827A5-38BD-4AD0-9833-92393568CA94}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABEE16A-F06D-4CDA-A89D-E56D66FA11D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34669" yWindow="-109" windowWidth="23040" windowHeight="13898" xr2:uid="{BC9F9AC6-E6B5-4E26-8DC4-44951FDC5054}"/>
   </bookViews>
@@ -968,11 +968,12 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>